<commit_message>
Arreglando bases de distritos y tribunales
</commit_message>
<xml_diff>
--- a/Bases_de_Rama_Judicial-DEA.xlsx
+++ b/Bases_de_Rama_Judicial-DEA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="24000" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="24000" windowHeight="9216" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="circuito" sheetId="5" r:id="rId1"/>
@@ -490,12 +490,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,13 +531,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,8 +538,19 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Millares [0]" xfId="3" builtinId="6"/>
     <cellStyle name="Millares [0] 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -828,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -862,19 +867,19 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="14">
         <v>360</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="14">
         <v>70</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="14">
         <v>716</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="14">
         <v>2</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="15">
         <f>SUM(B2,D2)</f>
         <v>1076</v>
       </c>
@@ -883,19 +888,19 @@
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="14">
         <v>240</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="14">
         <v>81</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="14">
         <v>430</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <v>6</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="15">
         <f t="shared" ref="F3:F39" si="0">SUM(B3,D3)</f>
         <v>670</v>
       </c>
@@ -904,19 +909,19 @@
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>68</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="14">
         <v>33</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="14">
         <v>102</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="14">
         <v>2</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="15">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
@@ -925,19 +930,19 @@
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>617</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="14">
         <v>270</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>1218</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <v>15</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="15">
         <f t="shared" si="0"/>
         <v>1835</v>
       </c>
@@ -946,19 +951,19 @@
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>2926</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="14">
         <v>1468</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>7632</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <v>65</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="15">
         <f t="shared" si="0"/>
         <v>10558</v>
       </c>
@@ -967,19 +972,19 @@
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>434</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="14">
         <v>225</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>553</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>15</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="15">
         <f t="shared" si="0"/>
         <v>987</v>
       </c>
@@ -988,19 +993,19 @@
       <c r="A8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="14">
         <v>107</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="14">
         <v>33</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>221</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>3</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="15">
         <f t="shared" si="0"/>
         <v>328</v>
       </c>
@@ -1009,19 +1014,19 @@
       <c r="A9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="14">
         <v>352</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="14">
         <v>122</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="14">
         <v>592</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>3</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="15">
         <f t="shared" si="0"/>
         <v>944</v>
       </c>
@@ -1030,19 +1035,19 @@
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
         <v>978</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="14">
         <v>389</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="14">
         <v>2462</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>21</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="15">
         <f t="shared" si="0"/>
         <v>3440</v>
       </c>
@@ -1051,19 +1056,19 @@
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="14">
         <v>554</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="14">
         <v>410</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="14">
         <v>1699</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="14">
         <v>15</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="15">
         <f t="shared" si="0"/>
         <v>2253</v>
       </c>
@@ -1072,19 +1077,19 @@
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="14">
         <v>317</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="14">
         <v>102</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="14">
         <v>1055</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <v>10</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="15">
         <f t="shared" si="0"/>
         <v>1372</v>
       </c>
@@ -1093,19 +1098,19 @@
       <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="14">
         <v>47</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="14">
         <v>8</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="14">
         <v>82</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>3</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="15">
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
@@ -1114,19 +1119,19 @@
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="14">
         <v>600</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="14">
         <v>187</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="14">
         <v>1151</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="14">
         <v>4</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="15">
         <f t="shared" si="0"/>
         <v>1751</v>
       </c>
@@ -1135,19 +1140,19 @@
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="14">
         <v>43</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="14">
         <v>11</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="14">
         <v>144</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="14">
         <v>3</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="15">
         <f t="shared" si="0"/>
         <v>187</v>
       </c>
@@ -1156,19 +1161,19 @@
       <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="14">
         <v>534</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="14">
         <v>173</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="14">
         <v>1251</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="14">
         <v>12</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="15">
         <f t="shared" si="0"/>
         <v>1785</v>
       </c>
@@ -1177,19 +1182,19 @@
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="14">
         <v>4</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="14">
         <v>4</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="14">
         <v>10</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="14">
         <v>1</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1198,19 +1203,19 @@
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="14">
         <v>259</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="14">
         <v>55</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="14">
         <v>627</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="14">
         <v>8</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="15">
         <f t="shared" si="0"/>
         <v>886</v>
       </c>
@@ -1219,19 +1224,19 @@
       <c r="A19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="14">
         <v>1247</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="14">
         <v>705</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="14">
         <v>3409</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="14">
         <v>36</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="15">
         <f t="shared" si="0"/>
         <v>4656</v>
       </c>
@@ -1240,19 +1245,19 @@
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="14">
         <v>493</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="14">
         <v>275</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="14">
         <v>407</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="14">
         <v>2</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="15">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
@@ -1261,19 +1266,19 @@
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="14">
         <v>309</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="14">
         <v>121</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="14">
         <v>672</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="14">
         <v>7</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="15">
         <f t="shared" si="0"/>
         <v>981</v>
       </c>
@@ -1282,19 +1287,19 @@
       <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="14">
         <v>406</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="14">
         <v>110</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="14">
         <v>1079</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="14">
         <v>9</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="15">
         <f t="shared" si="0"/>
         <v>1485</v>
       </c>
@@ -1303,19 +1308,19 @@
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="14">
         <v>30</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="14">
         <v>24</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="14">
         <v>75</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="14">
         <v>1</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="15">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
@@ -1324,19 +1329,19 @@
       <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="14">
         <v>485</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="14">
         <v>776</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="14">
         <v>1056</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="14">
         <v>9</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="15">
         <f t="shared" si="0"/>
         <v>1541</v>
       </c>
@@ -1345,19 +1350,19 @@
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="14">
         <v>238</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="14">
         <v>114</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="14">
         <v>559</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="14">
         <v>7</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="15">
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
@@ -1366,19 +1371,19 @@
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="14">
         <v>790</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="14">
         <v>397</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="14">
         <v>2281</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="14">
         <v>10</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="15">
         <f t="shared" si="0"/>
         <v>3071</v>
       </c>
@@ -1387,19 +1392,19 @@
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="14">
         <v>371</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="14">
         <v>64</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="14">
         <v>593</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="14">
         <v>4</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="15">
         <f t="shared" si="0"/>
         <v>964</v>
       </c>
@@ -1408,19 +1413,19 @@
       <c r="A28" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="14">
         <v>148</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="14">
         <v>43</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="14">
         <v>443</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="14">
         <v>3</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="15">
         <f t="shared" si="0"/>
         <v>591</v>
       </c>
@@ -1429,19 +1434,19 @@
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="14">
         <v>34</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="14">
         <v>13</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="14">
         <v>101</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="14">
         <v>1</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="15">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
@@ -1450,19 +1455,19 @@
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="14">
         <v>162</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="14">
         <v>51</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="14">
         <v>139</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="14">
         <v>3</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="15">
         <f t="shared" si="0"/>
         <v>301</v>
       </c>
@@ -1471,19 +1476,19 @@
       <c r="A31" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="14">
         <v>323</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="14">
         <v>129</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="14">
         <v>210</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="16">
         <v>7</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="15">
         <f t="shared" si="0"/>
         <v>533</v>
       </c>
@@ -1492,19 +1497,19 @@
       <c r="A32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="14">
         <v>267</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="14">
         <v>181</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="14">
         <v>774</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="14">
         <v>8</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="15">
         <f t="shared" si="0"/>
         <v>1041</v>
       </c>
@@ -1513,19 +1518,19 @@
       <c r="A33" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="14">
         <v>243</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="14">
         <v>153</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="14">
         <v>549</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="14">
         <v>9</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="15">
         <f t="shared" si="0"/>
         <v>792</v>
       </c>
@@ -1534,19 +1539,19 @@
       <c r="A34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="14">
         <v>180</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="14">
         <v>159</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="14">
         <v>327</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="14">
         <v>15</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="15">
         <f t="shared" si="0"/>
         <v>507</v>
       </c>
@@ -1555,19 +1560,19 @@
       <c r="A35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="14">
         <v>102</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="14">
         <v>38</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="14">
         <v>219</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="14">
         <v>2</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="15">
         <f t="shared" si="0"/>
         <v>321</v>
       </c>
@@ -1576,19 +1581,19 @@
       <c r="A36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="14">
         <v>631</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="14">
         <v>272</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="14">
         <v>1235</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="14">
         <v>8</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="15">
         <f t="shared" si="0"/>
         <v>1866</v>
       </c>
@@ -1597,19 +1602,19 @@
       <c r="A37" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="14">
         <v>427</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="14">
         <v>378</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="14">
         <v>894</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="14">
         <v>9</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F37" s="15">
         <f t="shared" si="0"/>
         <v>1321</v>
       </c>
@@ -1618,19 +1623,19 @@
       <c r="A38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="14">
         <v>124</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="14">
         <v>22</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="14">
         <v>319</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="14">
         <v>2</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="15">
         <f t="shared" si="0"/>
         <v>443</v>
       </c>
@@ -1639,19 +1644,19 @@
       <c r="A39" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="14">
         <v>28</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="14">
         <v>23</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="14">
         <v>32</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="14">
         <v>3</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="15">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1680,56 +1685,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="18">
         <v>2016</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1764,12 +1769,12 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1787,10 +1792,10 @@
       <c r="E9" s="1">
         <v>6</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1808,10 +1813,10 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1829,10 +1834,10 @@
       <c r="E11" s="1">
         <v>15</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2526,56 +2531,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="18">
         <v>2016</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2648,11 +2653,11 @@
       <c r="E10" s="8">
         <v>15</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -2670,9 +2675,9 @@
       <c r="E11" s="8">
         <v>15</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -2690,9 +2695,9 @@
       <c r="E12" s="8">
         <v>19</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -2710,9 +2715,9 @@
       <c r="E13" s="8">
         <v>8</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -3132,7 +3137,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3165,19 +3170,19 @@
       <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="19">
         <v>1349</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="19">
         <v>743</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="19">
         <v>3628</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="19">
         <v>38</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="20">
         <f>SUM(B2,D2)</f>
         <v>4977</v>
       </c>
@@ -3188,19 +3193,19 @@
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="19">
         <v>360</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="19">
         <v>70</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="19">
         <v>716</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="19">
         <v>2</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="20">
         <f t="shared" ref="F3:F27" si="0">SUM(B3,D3)</f>
         <v>1076</v>
       </c>
@@ -3211,19 +3216,19 @@
       <c r="A4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="19">
         <v>617</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="19">
         <v>270</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="19">
         <v>1218</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="19">
         <v>15</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="20">
         <f t="shared" si="0"/>
         <v>1835</v>
       </c>
@@ -3234,19 +3239,19 @@
       <c r="A5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="19">
         <v>554</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="19">
         <v>410</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="19">
         <v>1699</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="19">
         <v>15</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="20">
         <f t="shared" si="0"/>
         <v>2253</v>
       </c>
@@ -3257,19 +3262,19 @@
       <c r="A6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="19">
         <v>503</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="19">
         <v>288</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="19">
         <v>537</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="19">
         <v>19</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="20">
         <f t="shared" si="0"/>
         <v>1040</v>
       </c>
@@ -3280,19 +3285,19 @@
       <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="19">
         <v>259</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="19">
         <v>55</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="19">
         <v>627</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="19">
         <v>8</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="20">
         <f t="shared" si="0"/>
         <v>886</v>
       </c>
@@ -3303,19 +3308,19 @@
       <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="19">
         <v>600</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="19">
         <v>187</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="19">
         <v>1151</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="19">
         <v>4</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="20">
         <f t="shared" si="0"/>
         <v>1751</v>
       </c>
@@ -3326,19 +3331,19 @@
       <c r="A9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="19">
         <v>124</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="19">
         <v>22</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="19">
         <v>319</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="19">
         <v>2</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="20">
         <f t="shared" si="0"/>
         <v>443</v>
       </c>
@@ -3349,19 +3354,19 @@
       <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="19">
         <v>790</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="19">
         <v>397</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="19">
         <v>2281</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="19">
         <v>10</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="20">
         <f t="shared" si="0"/>
         <v>3071</v>
       </c>
@@ -3372,19 +3377,19 @@
       <c r="A11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="19">
         <v>631</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="19">
         <v>272</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="19">
         <v>1235</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="19">
         <v>8</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="20">
         <f t="shared" si="0"/>
         <v>1866</v>
       </c>
@@ -3395,19 +3400,19 @@
       <c r="A12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="19">
         <v>371</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="19">
         <v>64</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="19">
         <v>593</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="19">
         <v>4</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="20">
         <f t="shared" si="0"/>
         <v>964</v>
       </c>
@@ -3418,19 +3423,19 @@
       <c r="A13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="19">
         <v>309</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="19">
         <v>121</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="19">
         <v>672</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="19">
         <v>7</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="20">
         <f t="shared" si="0"/>
         <v>981</v>
       </c>
@@ -3441,19 +3446,19 @@
       <c r="A14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="19">
         <v>3048</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="19">
         <v>1514</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="19">
         <v>7900</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="19">
         <v>75</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="20">
         <f t="shared" si="0"/>
         <v>10948</v>
       </c>
@@ -3464,19 +3469,19 @@
       <c r="A15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="19">
         <v>148</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="19">
         <v>43</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="19">
         <v>443</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="19">
         <v>3</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="20">
         <f t="shared" si="0"/>
         <v>591</v>
       </c>
@@ -3487,19 +3492,19 @@
       <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="19">
         <v>406</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="19">
         <v>110</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="19">
         <v>1079</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="19">
         <v>9</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="20">
         <f t="shared" si="0"/>
         <v>1485</v>
       </c>
@@ -3510,19 +3515,19 @@
       <c r="A17" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="19">
         <v>267</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="19">
         <v>181</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="19">
         <v>774</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="19">
         <v>8</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="20">
         <f t="shared" si="0"/>
         <v>1041</v>
       </c>
@@ -3533,19 +3538,19 @@
       <c r="A18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="19">
         <v>427</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="19">
         <v>378</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="19">
         <v>894</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="19">
         <v>9</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="20">
         <f t="shared" si="0"/>
         <v>1321</v>
       </c>
@@ -3556,19 +3561,19 @@
       <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="19">
         <v>978</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="19">
         <v>1051</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="19">
         <v>1463</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="19">
         <v>11</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="20">
         <f t="shared" si="0"/>
         <v>2441</v>
       </c>
@@ -3579,19 +3584,19 @@
       <c r="A20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="19">
         <v>347</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="19">
         <v>126</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="19">
         <v>1130</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="19">
         <v>11</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="20">
         <f t="shared" si="0"/>
         <v>1477</v>
       </c>
@@ -3602,19 +3607,19 @@
       <c r="A21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="19">
         <v>240</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="19">
         <v>81</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="19">
         <v>430</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="19">
         <v>6</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="20">
         <f t="shared" si="0"/>
         <v>670</v>
       </c>
@@ -3625,19 +3630,19 @@
       <c r="A22" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="19">
         <v>238</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="19">
         <v>114</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="19">
         <v>559</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="19">
         <v>7</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="20">
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
@@ -3648,19 +3653,19 @@
       <c r="A23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="19">
         <v>34</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="19">
         <v>13</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="19">
         <v>101</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="19">
         <v>1</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="20">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
@@ -3671,19 +3676,19 @@
       <c r="A24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="19">
         <v>664</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="19">
         <v>309</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="19">
         <v>794</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="19">
         <v>20</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="20">
         <f t="shared" si="0"/>
         <v>1458</v>
       </c>
@@ -3694,19 +3699,19 @@
       <c r="A25" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="19">
         <v>243</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="19">
         <v>153</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="19">
         <v>549</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="19">
         <v>9</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="20">
         <f t="shared" si="0"/>
         <v>792</v>
       </c>
@@ -3717,19 +3722,19 @@
       <c r="A26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="19">
         <v>534</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="19">
         <v>173</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="19">
         <v>1251</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="19">
         <v>12</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="20">
         <f t="shared" si="0"/>
         <v>1785</v>
       </c>
@@ -3740,19 +3745,19 @@
       <c r="A27" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="19">
         <v>1437</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="19">
         <v>544</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="19">
         <v>3275</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="19">
         <v>29</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="20">
         <f t="shared" si="0"/>
         <v>4712</v>
       </c>
@@ -3779,56 +3784,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="18">
         <v>2016</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -4462,8 +4467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4496,19 +4501,19 @@
       <c r="A2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="14">
         <v>1360</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="14">
         <v>680</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="14">
         <v>1105</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="14">
         <v>15</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="15">
         <f>SUM(B2,D2)</f>
         <v>2465</v>
       </c>
@@ -4519,19 +4524,19 @@
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="14">
         <v>98</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="14">
         <v>126</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="14">
         <v>114</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="14">
         <v>3</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="15">
         <f t="shared" ref="F3:F27" si="0">SUM(B3,D3)</f>
         <v>212</v>
       </c>
@@ -4542,19 +4547,19 @@
       <c r="A4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="14">
         <v>312</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="14">
         <v>332</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="14">
         <v>481</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="14">
         <v>9</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="15">
         <f t="shared" si="0"/>
         <v>793</v>
       </c>
@@ -4565,19 +4570,19 @@
       <c r="A5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="14">
         <v>460</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="14">
         <v>195</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="14">
         <v>559</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="14">
         <v>6</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="15">
         <f t="shared" si="0"/>
         <v>1019</v>
       </c>
@@ -4588,19 +4593,19 @@
       <c r="A6" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="14">
         <v>316</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="14">
         <v>239</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="14">
         <v>337</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="14">
         <v>6</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="15">
         <f t="shared" si="0"/>
         <v>653</v>
       </c>
@@ -4611,19 +4616,19 @@
       <c r="A7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="14">
         <v>221</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="14">
         <v>150</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="14">
         <v>194</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="14">
         <v>6</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="15">
         <f t="shared" si="0"/>
         <v>415</v>
       </c>
@@ -4634,19 +4639,19 @@
       <c r="A8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="14">
         <v>398</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="14">
         <v>244</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="14">
         <v>614</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="14">
         <v>4</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="15">
         <f t="shared" si="0"/>
         <v>1012</v>
       </c>
@@ -4657,19 +4662,19 @@
       <c r="A9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="14">
         <v>100</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="14">
         <v>90</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="14">
         <v>124</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="14">
         <v>3</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="15">
         <f t="shared" si="0"/>
         <v>224</v>
       </c>
@@ -4680,19 +4685,19 @@
       <c r="A10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="14">
         <v>440</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="14">
         <v>314</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="14">
         <v>631</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="14">
         <v>5</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="15">
         <f t="shared" si="0"/>
         <v>1071</v>
       </c>
@@ -4703,19 +4708,19 @@
       <c r="A11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="14">
         <v>416</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="14">
         <v>265</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="14">
         <v>222</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="14">
         <v>4</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="15">
         <f t="shared" si="0"/>
         <v>638</v>
       </c>
@@ -4726,19 +4731,19 @@
       <c r="A12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="14">
         <v>152</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="14">
         <v>72</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="14">
         <v>196</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="14">
         <v>3</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="15">
         <f t="shared" si="0"/>
         <v>348</v>
       </c>
@@ -4749,19 +4754,19 @@
       <c r="A13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="14">
         <v>131</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="14">
         <v>83</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="14">
         <v>340</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="14">
         <v>4</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="15">
         <f t="shared" si="0"/>
         <v>471</v>
       </c>
@@ -4772,19 +4777,19 @@
       <c r="A14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="14">
         <v>2059</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="14">
         <v>1477</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="14">
         <v>1670</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="14">
         <v>9</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="15">
         <f t="shared" si="0"/>
         <v>3729</v>
       </c>
@@ -4795,19 +4800,19 @@
       <c r="A15" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="14">
         <v>49</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="14">
         <v>70</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="14">
         <v>131</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="14">
         <v>3</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="15">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
@@ -4818,19 +4823,19 @@
       <c r="A16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="14">
         <v>178</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="14">
         <v>216</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="14">
         <v>308</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="14">
         <v>6</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="15">
         <f t="shared" si="0"/>
         <v>486</v>
       </c>
@@ -4841,19 +4846,19 @@
       <c r="A17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="14">
         <v>157</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="14">
         <v>116</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="14">
         <v>349</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="14">
         <v>4</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>506</v>
       </c>
@@ -4864,19 +4869,19 @@
       <c r="A18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="14">
         <v>767</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="14">
         <v>240</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="14">
         <v>772</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="14">
         <v>5</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="15">
         <f t="shared" si="0"/>
         <v>1539</v>
       </c>
@@ -4887,19 +4892,19 @@
       <c r="A19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="14">
         <v>550</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="14">
         <v>402</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="14">
         <v>713</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="14">
         <v>6</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="15">
         <f t="shared" si="0"/>
         <v>1263</v>
       </c>
@@ -4910,19 +4915,19 @@
       <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="14">
         <v>333</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="14">
         <v>195</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="14">
         <v>342</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="14">
         <v>5</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="15">
         <f t="shared" si="0"/>
         <v>675</v>
       </c>
@@ -4933,19 +4938,19 @@
       <c r="A21" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="14">
         <v>331</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="14">
         <v>173</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="14">
         <v>190</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="14">
         <v>5</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="15">
         <f t="shared" si="0"/>
         <v>521</v>
       </c>
@@ -4956,19 +4961,19 @@
       <c r="A22" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="14">
         <v>281</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="14">
         <v>138</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="14">
         <v>278</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="14">
         <v>4</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="15">
         <f t="shared" si="0"/>
         <v>559</v>
       </c>
@@ -4979,19 +4984,19 @@
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="14">
         <v>19</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="14">
         <v>28</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="14">
         <v>82</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="14">
         <v>3</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="15">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
@@ -5002,19 +5007,19 @@
       <c r="A24" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="14">
         <v>396</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="14">
         <v>264</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="14">
         <v>578</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="14">
         <v>6</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="15">
         <f t="shared" si="0"/>
         <v>974</v>
       </c>
@@ -5025,19 +5030,19 @@
       <c r="A25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="14">
         <v>109</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="14">
         <v>192</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="14">
         <v>329</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="14">
         <v>4</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="15">
         <f t="shared" si="0"/>
         <v>438</v>
       </c>
@@ -5048,19 +5053,19 @@
       <c r="A26" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="14">
         <v>282</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="14">
         <v>196</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="14">
         <v>257</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="14">
         <v>6</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="15">
         <f t="shared" si="0"/>
         <v>539</v>
       </c>
@@ -5071,19 +5076,19 @@
       <c r="A27" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="14">
         <v>803</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="14">
         <v>195</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="14">
         <v>1459</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="14">
         <v>12</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="15">
         <f t="shared" si="0"/>
         <v>2262</v>
       </c>

</xml_diff>